<commit_message>
Mise a jour avec Serveur
</commit_message>
<xml_diff>
--- a/uploads/Blending Operations Compliance exploitation phase stage 1.xlsx
+++ b/uploads/Blending Operations Compliance exploitation phase stage 1.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="12240" windowHeight="7995"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="12240" windowHeight="7935"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -31,7 +31,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Ernst &amp; Young:</t>
+          <t xml:space="preserve">Road Map of the Mbalam Mining Convention - Exploitation Phase Blending Operations :
+</t>
         </r>
         <r>
           <rPr>
@@ -41,15 +42,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Pursuant to article 1 of the Convention, Blending Operations means the operations relating to the industrial process whereby Nabeba Ore (iron ore produced from the area covered by the Nabeba Permit in the Republic of Congo), an Other Ores (other than Nabeba Ore) (with the consent of the State) are blended with Mbalam Ore, which operations are carried out in accordance with the terms and conditions of the Convention, the Blending Agreement, and the Monitoring Agreement - Blending or such similar agreements.
-To recall, Blending Operations shall be carried out by the Mineral Terminal Project Company (see the definition of the Mineral Terminal Project Company according to which the Mineral Terminal Project is in charge both of the Mineral Terminal Operations and the Blending Operations). However, we would like to draw your attention to the fact that article 16.1(c) of the Convention seems to indicate that the Mine Project Company can also conduct Blending Operations within the Mineral Terminal Area under the Conditions set forth in the Mineral Terminal Services Agreement. 
-It results from the definition of Blending Operations that such operations shall be carried out in accordance with the provisions of:
-- the Convention;
-- the Blending Agreement to be concluded between the Mine Project Company, Congo Iron and the Mineral Terminal Project Company;
-- the Mineral Terminal Agreement (see the definition if this agreement)
-- the Monitoring Agreement - Blending 
-- the Mineral Terminal Services Agreement. 
-</t>
+The Mineral Terminal Services Agreement is the services agreement concluded between the Mineral Terminal Project Company and either the Mine Project Company or a Third Party contracting to utilise the services of the Mineral Terminal Project Company which may include a description of the tariff to be charged by the Mineral Terminal Project Company (article 1 of the Convention).
+Pursuant to article 16.1(c) of the Convention, the Mineral Terminal Service Agreement provide and set the framework of the conditions for the conduct by the Mine Project Company of the Blending Operations within the Mineral Terminal Area. Reference is therefore made to this agreement with respect to the requirements and compliances to be satified within the course of Blending Operations. This convention must be concluded prior to and as a Condition Precedent to the entry into force of the Convention. </t>
         </r>
       </text>
     </comment>
@@ -79,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,6 +96,56 @@
           <t xml:space="preserve">
 The Blending Agreement means the agreement relating to the Blending of Mbalam Ore from the territory covered by the Nabeba Permit to be concluded between the Mine Project Company, Congo Iron and the Mineral Terminal Project Company which will establish the provisions regarding the blending of Mbalam Ore and Nabeba Ore.
 As per article 16.1 (c) of the Convention, the Blending Agreement provides for, with the Mineral Terminal Services Agreement, the framework of the Conditions of conduct by the Mine Project Company of Blending Operations within the Mineral Terminal Area. This convention must be concluded prior to and as a Condition Precedent of the entry into force of the Convention. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Road Map of the Mbalam Mining Convention - Exploitation Phase Blending Operations :
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The Blending Agreement means the agreement relating to the Blending of Mbalam Ore from the territory covered by the Nabeba Permit to be concluded between the Mine Project Company, Congo Iron and the Mineral Terminal Project Company which will establish the provisions regarding the blending of Mbalam Ore and Nabeba Ore.
+As per article 16.1 (c) of the Convention, the Blending Agreement provides for, with the Mineral Terminal Services Agreement, the framework of the Conditions of conduct by the Mine Project Company of Blending Operations within the Mineral Terminal Area. This convention must be concluded prior to and as a Condition Precedent of the entry into force of the Convention. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Road Map of the Mbalam Mining Convention - Exploitation Phase Blending Operations :</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+As per article 1 of the Convention, Monitoriing Agreement -Blending means the agreement relating to the rights of the State to review the Blending Operations and the right for the Mine Project Company and Congo Iron to be protected from discriminatory or disproportionate treatment with regard to Blending Operations. This Contract shall therefore be concluded between the State, Cam Iron, Congo Iron and the Mineral Terminal Project Company prior to and as a Condition Precedent of the entry into force of the Convention. </t>
         </r>
       </text>
     </comment>
@@ -134,7 +178,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>Due date for action</t>
   </si>
@@ -163,9 +207,6 @@
     <t>Pending</t>
   </si>
   <si>
-    <t>Monitoring Items / Categories</t>
-  </si>
-  <si>
     <t>Required action or operation (what need to be done)</t>
   </si>
   <si>
@@ -179,9 +220,6 @@
   </si>
   <si>
     <t>State authority accountable for compliance</t>
-  </si>
-  <si>
-    <t>Blending Operations Compliance</t>
   </si>
   <si>
     <t>Comply with the provisions of the Mineral Terminal Services Agreement (article 16.1(b) and (c) of the Convention)</t>
@@ -231,16 +269,19 @@
   </si>
   <si>
     <t>The requirements of the Monitoring Agreement-Blending duly satisfied</t>
+  </si>
+  <si>
+    <t>Conditions precedent to be satisfied</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -254,7 +295,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -291,7 +331,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -306,8 +346,8 @@
       <right style="thick">
         <color theme="0" tint="-0.499984740745262"/>
       </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom style="thick">
         <color theme="0" tint="-0.499984740745262"/>
@@ -321,42 +361,10 @@
       <right style="thick">
         <color theme="0" tint="-0.499984740745262"/>
       </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -375,8 +383,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
       <right style="thick">
         <color theme="0" tint="-0.499984740745262"/>
@@ -393,6 +401,19 @@
       <left style="thick">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
+      <right style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -405,8 +426,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
+      <left style="thick">
+        <color theme="0" tint="-0.499984740745262"/>
       </left>
       <right style="thick">
         <color theme="0" tint="-0.499984740745262"/>
@@ -438,79 +459,66 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,91 +533,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1085850</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 41"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="15592425" cy="1733550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>1085850</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 41"/>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1" noTextEdit="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="15592425" cy="1733550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -683,6 +608,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -717,6 +643,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -892,276 +819,227 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="4" width="33.28515625" customWidth="1"/>
-    <col min="5" max="10" width="15.7109375" customWidth="1"/>
-    <col min="11" max="11" width="31.5703125" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" customWidth="1"/>
-    <col min="14" max="14" width="22" customWidth="1"/>
-    <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="3" max="6" width="17.42578125" customWidth="1"/>
+    <col min="7" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="31.5703125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="22" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" ht="33" customHeight="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+    <row r="1" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:13" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
     </row>
-    <row r="2" spans="1:13" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
+    <row r="4" spans="1:13" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" ht="72" customHeight="1" thickBot="1"/>
-    <row r="4" spans="1:13" ht="46.5" customHeight="1" thickBot="1">
-      <c r="A4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="6" t="s">
+    <row r="5" spans="1:13" s="9" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" ht="79.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="B6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="12"/>
+      <c r="K6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6" s="15"/>
     </row>
-    <row r="5" spans="1:13" s="8" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="12"/>
+    <row r="7" spans="1:13" ht="75.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="15"/>
     </row>
-    <row r="6" spans="1:13" ht="79.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="19" t="s">
+    <row r="8" spans="1:13" ht="81" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="21"/>
+      <c r="I8" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="18"/>
+      <c r="K8" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="21"/>
+      <c r="M8" s="22"/>
     </row>
-    <row r="7" spans="1:13" ht="75.75" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="21"/>
-    </row>
-    <row r="8" spans="1:13" ht="81" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="26" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" s="23"/>
-      <c r="K8" s="17" t="s">
-        <v>31</v>
-      </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="25"/>
-    </row>
-    <row r="20" ht="46.5" customHeight="1"/>
-    <row r="24" ht="76.5" customHeight="1"/>
-    <row r="28" ht="16.5" customHeight="1"/>
-    <row r="30" ht="31.5" customHeight="1"/>
-    <row r="35" ht="46.5" customHeight="1"/>
-    <row r="38" ht="31.5" customHeight="1"/>
-    <row r="43" ht="46.5" customHeight="1"/>
-    <row r="45" ht="61.5" customHeight="1"/>
-    <row r="49" ht="16.5" customHeight="1"/>
-    <row r="51" ht="46.5" customHeight="1"/>
-    <row r="54" ht="16.5" customHeight="1"/>
-    <row r="58" ht="31.5" customHeight="1"/>
-    <row r="62" ht="31.5" customHeight="1"/>
-    <row r="66" ht="31.5" customHeight="1"/>
-    <row r="70" ht="31.5" customHeight="1"/>
-    <row r="74" ht="16.5" customHeight="1"/>
-    <row r="79" ht="16.5" customHeight="1"/>
-    <row r="84" ht="31.5" customHeight="1"/>
-    <row r="90" ht="31.5" customHeight="1"/>
-    <row r="92" ht="31.5" customHeight="1"/>
-    <row r="94" ht="31.5" customHeight="1"/>
-    <row r="96" ht="16.5" customHeight="1"/>
-    <row r="97" ht="20.100000000000001" customHeight="1"/>
-    <row r="98" ht="20.100000000000001" customHeight="1"/>
-    <row r="99" ht="17.25" customHeight="1"/>
-    <row r="100" ht="20.100000000000001" customHeight="1"/>
-    <row r="101" ht="20.25" customHeight="1"/>
-    <row r="102" ht="18.75" customHeight="1"/>
-    <row r="103" ht="36" customHeight="1"/>
-    <row r="104" ht="28.5" customHeight="1"/>
-    <row r="105" ht="25.5" customHeight="1"/>
-    <row r="106" ht="27.75" customHeight="1"/>
-    <row r="107" ht="18" customHeight="1"/>
-    <row r="108" ht="22.5" customHeight="1"/>
-    <row r="109" ht="76.5" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A3:I3"/>
     <mergeCell ref="L6:L8"/>
+    <mergeCell ref="F4:F5"/>
+    <mergeCell ref="G4:G5"/>
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:J4"/>
     <mergeCell ref="K4:K5"/>
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="M4:M5"/>
-    <mergeCell ref="A6:A8"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
-    <mergeCell ref="F4:F5"/>
-    <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Chargement des tâches phases exploitation 1
- Chargement des fichiers
- Trie des tâches en fonction de la catégories
-Suppression de l'adresse juan@camiron.net
- suppression du bouton de comptage des notifications
</commit_message>
<xml_diff>
--- a/uploads/Blending Operations Compliance exploitation phase stage 1.xlsx
+++ b/uploads/Blending Operations Compliance exploitation phase stage 1.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="12240" windowHeight="7935"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="15195" windowHeight="8130"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -180,9 +180,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
+    <t>Conditions precedent to be satisfied</t>
+  </si>
+  <si>
+    <t>Required action or operation (what need to be done)</t>
+  </si>
+  <si>
+    <t>Date for compliance (timeframe, deadline)</t>
+  </si>
+  <si>
+    <t>Party action accountable for compliance</t>
+  </si>
+  <si>
+    <t>Person in charge</t>
+  </si>
+  <si>
     <t>Due date for action</t>
   </si>
   <si>
+    <t>State authority accountable for compliance</t>
+  </si>
+  <si>
     <t>Status</t>
   </si>
   <si>
@@ -204,31 +222,16 @@
     <t>State</t>
   </si>
   <si>
+    <t>Comply with the provisions of the Mineral Terminal Services Agreement (article 16.1(b) and (c) of the Convention)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the term of the Mineral Terminal Services Agreement </t>
+  </si>
+  <si>
+    <t>Mine Project Company/Mineral Terminal Project Company</t>
+  </si>
+  <si>
     <t>Pending</t>
-  </si>
-  <si>
-    <t>Required action or operation (what need to be done)</t>
-  </si>
-  <si>
-    <t>Date for compliance (timeframe, deadline)</t>
-  </si>
-  <si>
-    <t>Party action accountable for compliance</t>
-  </si>
-  <si>
-    <t>Person in charge</t>
-  </si>
-  <si>
-    <t>State authority accountable for compliance</t>
-  </si>
-  <si>
-    <t>Comply with the provisions of the Mineral Terminal Services Agreement (article 16.1(b) and (c) of the Convention)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">During the term of the Mineral Terminal Services Agreement </t>
-  </si>
-  <si>
-    <t>Mine Project Company/Mineral Terminal Project Company</t>
   </si>
   <si>
     <t>The Mineral Terminal
@@ -269,9 +272,6 @@
   </si>
   <si>
     <t>The requirements of the Monitoring Agreement-Blending duly satisfied</t>
-  </si>
-  <si>
-    <t>Conditions precedent to be satisfied</t>
   </si>
 </sst>
 </file>
@@ -279,29 +279,15 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -316,22 +302,22 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -340,117 +326,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top/>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thick">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -459,66 +344,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -534,7 +386,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -820,189 +672,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A4:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="31.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="22" customWidth="1"/>
-    <col min="13" max="13" width="14.42578125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="36" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:13" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="2"/>
+    </row>
+    <row r="6" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" s="6"/>
+    </row>
+    <row r="7" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="8"/>
+      <c r="M7" s="6"/>
+    </row>
+    <row r="8" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" s="9" customFormat="1" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="8"/>
-    </row>
-    <row r="6" spans="1:13" ht="79.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" s="15"/>
-    </row>
-    <row r="7" spans="1:13" ht="75.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="15"/>
-    </row>
-    <row r="8" spans="1:13" ht="81" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="L8" s="21"/>
-      <c r="M8" s="22"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="A3:I3"/>
+  <mergeCells count="13">
     <mergeCell ref="L6:L8"/>
-    <mergeCell ref="F4:F5"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="I4:J4"/>
@@ -1014,9 +841,10 @@
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:E5"/>
+    <mergeCell ref="F4:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -1027,7 +855,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1039,7 +867,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>